<commit_message>
Commit for Credential Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Credentials.xlsx
+++ b/src/test/resources/Credentials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -83,13 +83,19 @@
     <t>TC001_RegisterUser</t>
   </si>
   <si>
-    <t>Duchess</t>
-  </si>
-  <si>
     <t>Gowtham</t>
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Lieutenant Colonel</t>
+  </si>
+  <si>
+    <t>Provisional</t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
 </sst>
 </file>
@@ -458,13 +464,13 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
@@ -551,21 +557,29 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E2" s="5">
         <v>9445929408</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="F2" s="5">
+        <v>1998</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="5">
+        <v>30</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -580,10 +594,12 @@
       <c r="U2" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
-      <formula1>1</formula1>
-      <formula2>30</formula2>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"Mr,Mrs,Miss,Ms,Doctor,Captain,Duchess,Duke,Father,General,Lady,Lord,Lieutenant,Lieutenant Colonel,Major,Master,Professor,Reverend,Sir,Squire,Squadron Leader"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+      <formula1>"Full,Provisional"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes on radio button condition
</commit_message>
<xml_diff>
--- a/src/test/resources/Credentials.xlsx
+++ b/src/test/resources/Credentials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>May</t>
+  </si>
+  <si>
+    <t>1984</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,8 +571,8 @@
       <c r="E2" s="5">
         <v>9445929408</v>
       </c>
-      <c r="F2" s="5">
-        <v>1998</v>
+      <c r="F2" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Commit for AjaxElement Factory removal
</commit_message>
<xml_diff>
--- a/src/test/resources/Credentials.xlsx
+++ b/src/test/resources/Credentials.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Guru99Automation\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16344" windowHeight="3264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16344" windowHeight="6504"/>
   </bookViews>
   <sheets>
     <sheet name="testCaseData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -89,9 +85,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Lieutenant Colonel</t>
-  </si>
-  <si>
     <t>Provisional</t>
   </si>
   <si>
@@ -99,6 +92,45 @@
   </si>
   <si>
     <t>1984</t>
+  </si>
+  <si>
+    <t>Museum Curator</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Squadron Leader</t>
   </si>
 </sst>
 </file>
@@ -464,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:AC80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,15 +514,17 @@
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
     <col min="11" max="11" width="14.21875" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
+    <col min="13" max="13" width="29.88671875" customWidth="1"/>
+    <col min="14" max="14" width="42.44140625" customWidth="1"/>
     <col min="15" max="15" width="23.77734375" customWidth="1"/>
     <col min="16" max="16" width="18.109375" customWidth="1"/>
     <col min="17" max="17" width="14.21875" customWidth="1"/>
     <col min="18" max="18" width="23.77734375" customWidth="1"/>
+    <col min="29" max="29" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,13 +588,22 @@
       <c r="U1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA1">
+        <v>1</v>
+      </c>
+      <c r="AB1">
+        <v>1935</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -572,19 +615,23 @@
         <v>9445929408</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" s="5">
         <v>30</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="J2" s="5">
+        <v>7</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -595,15 +642,636 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>1936</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AB3">
+        <v>1937</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA4">
+        <v>4</v>
+      </c>
+      <c r="AB4">
+        <v>1938</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA5">
+        <v>5</v>
+      </c>
+      <c r="AB5">
+        <v>1939</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA6">
+        <v>6</v>
+      </c>
+      <c r="AB6">
+        <v>1940</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA7">
+        <v>7</v>
+      </c>
+      <c r="AB7">
+        <v>1941</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA8">
+        <v>8</v>
+      </c>
+      <c r="AB8">
+        <v>1942</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA9">
+        <v>9</v>
+      </c>
+      <c r="AB9">
+        <v>1943</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA10">
+        <v>10</v>
+      </c>
+      <c r="AB10">
+        <v>1944</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA11">
+        <v>11</v>
+      </c>
+      <c r="AB11">
+        <v>1945</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA12">
+        <v>12</v>
+      </c>
+      <c r="AB12">
+        <v>1946</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA13">
+        <v>13</v>
+      </c>
+      <c r="AB13">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA14">
+        <v>14</v>
+      </c>
+      <c r="AB14">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA15">
+        <v>15</v>
+      </c>
+      <c r="AB15">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA16">
+        <v>16</v>
+      </c>
+      <c r="AB16">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="17" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA17">
+        <v>17</v>
+      </c>
+      <c r="AB17">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="18" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA18">
+        <v>18</v>
+      </c>
+      <c r="AB18">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="19" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA19">
+        <v>19</v>
+      </c>
+      <c r="AB19">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="20" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA20">
+        <v>20</v>
+      </c>
+      <c r="AB20">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="21" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA21">
+        <v>21</v>
+      </c>
+      <c r="AB21">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="22" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA22">
+        <v>22</v>
+      </c>
+      <c r="AB22">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="23" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA23">
+        <v>23</v>
+      </c>
+      <c r="AB23">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="24" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA24">
+        <v>24</v>
+      </c>
+      <c r="AB24">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="25" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA25">
+        <v>25</v>
+      </c>
+      <c r="AB25">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="26" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA26">
+        <v>26</v>
+      </c>
+      <c r="AB26">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="27" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA27">
+        <v>27</v>
+      </c>
+      <c r="AB27">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="28" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA28">
+        <v>28</v>
+      </c>
+      <c r="AB28">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="29" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA29">
+        <v>29</v>
+      </c>
+      <c r="AB29">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="30" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA30">
+        <v>30</v>
+      </c>
+      <c r="AB30">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="31" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA31">
+        <v>31</v>
+      </c>
+      <c r="AB31">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="32" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA32">
+        <v>32</v>
+      </c>
+      <c r="AB32">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="33" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA33">
+        <v>33</v>
+      </c>
+      <c r="AB33">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="34" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA34">
+        <v>34</v>
+      </c>
+      <c r="AB34">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="35" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA35">
+        <v>35</v>
+      </c>
+      <c r="AB35">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="36" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA36">
+        <v>36</v>
+      </c>
+      <c r="AB36">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="37" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA37">
+        <v>37</v>
+      </c>
+      <c r="AB37">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="38" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA38">
+        <v>38</v>
+      </c>
+      <c r="AB38">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="39" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA39">
+        <v>39</v>
+      </c>
+      <c r="AB39">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="40" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA40">
+        <v>40</v>
+      </c>
+      <c r="AB40">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="41" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA41">
+        <v>41</v>
+      </c>
+      <c r="AB41">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="42" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA42">
+        <v>42</v>
+      </c>
+      <c r="AB42">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="43" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA43">
+        <v>43</v>
+      </c>
+      <c r="AB43">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="44" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA44">
+        <v>44</v>
+      </c>
+      <c r="AB44">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="45" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA45">
+        <v>45</v>
+      </c>
+      <c r="AB45">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="46" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA46">
+        <v>46</v>
+      </c>
+      <c r="AB46">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="47" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA47">
+        <v>47</v>
+      </c>
+      <c r="AB47">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="48" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA48">
+        <v>48</v>
+      </c>
+      <c r="AB48">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="49" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA49">
+        <v>49</v>
+      </c>
+      <c r="AB49">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="50" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA50">
+        <v>50</v>
+      </c>
+      <c r="AB50">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="51" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA51">
+        <v>51</v>
+      </c>
+      <c r="AB51">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="52" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA52">
+        <v>52</v>
+      </c>
+      <c r="AB52">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="53" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA53">
+        <v>53</v>
+      </c>
+      <c r="AB53">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="54" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA54">
+        <v>54</v>
+      </c>
+      <c r="AB54">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="55" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA55">
+        <v>55</v>
+      </c>
+      <c r="AB55">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="56" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA56">
+        <v>56</v>
+      </c>
+      <c r="AB56">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="57" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA57">
+        <v>57</v>
+      </c>
+      <c r="AB57">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="58" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA58">
+        <v>58</v>
+      </c>
+      <c r="AB58">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="59" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA59">
+        <v>59</v>
+      </c>
+      <c r="AB59">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="60" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA60">
+        <v>60</v>
+      </c>
+      <c r="AB60">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="61" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA61">
+        <v>61</v>
+      </c>
+      <c r="AB61">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="62" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA62">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA63">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="27:28" x14ac:dyDescent="0.3">
+      <c r="AA64">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA65">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA66">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA67">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA68">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA69">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA71">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA72">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA73">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA74">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA75">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA76">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA77">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA78">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA79">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA80">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"Mr,Mrs,Miss,Ms,Doctor,Captain,Duchess,Duke,Father,General,Lady,Lord,Lieutenant,Lieutenant Colonel,Major,Master,Professor,Reverend,Sir,Squire,Squadron Leader"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
       <formula1>"Full,Provisional"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>$AA$1:$AA$80</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+      <formula1>"Academic,Actor,Artist,Doctor,Librarian,Student,Accountant,Architect,Dentist,Economists,Writer,Engineer,Lawyer,Nurse,Phramacist,Physiotherapist,Psychologist,Scientist,Social worker,Statistican,Surgeon,Teacher,Math Professor,Bank Examiner,Museum Curator"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>$AB$1:$AB$61</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>$AC$1:$AC$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+      <formula1>$AA$1:$AA$31</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>